<commit_message>
make Unit test UIUX.U46_Open_SmartCombo.xlsx
</commit_message>
<xml_diff>
--- a/Lending/Document/UIUX.CIBER_UIUXIBMB-928/UIUX.U46_Open_SmartCombo.xlsx
+++ b/Lending/Document/UIUX.CIBER_UIUXIBMB-928/UIUX.U46_Open_SmartCombo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces_2018\DemoSAP_UI5_Git\SAPUI_DEMO\Lending\Document\UIUX.CIBER_UIUXIBMB-928\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD30A35C-856D-4D11-B24A-B5DDA1A449BC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D3B936C-CF4F-4C2F-8902-3C779E776598}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>TT</t>
   </si>
@@ -122,17 +122,129 @@
     <t xml:space="preserve">Open Smart Combo </t>
   </si>
   <si>
-    <t>GetMaxRateAndTermOnlineSaving Service</t>
-  </si>
-  <si>
-    <t>https://IP_HOST:PORT/cb/odata/services/onlinesavingservice/GetMaxRateAndTermOnlineSaving?SavingProductCode='TD6018'&amp;Currency='VND'&amp;AppliedDate='2018-01-01'&amp;BranchId='VN0010106'</t>
+    <t>OnlineSavingAccountTypes?SEARCH_TYPE=ALL_ONLINE_SAVING service</t>
+  </si>
+  <si>
+    <t>https://smp-srv:8081/cb/odata/services/onlinesavingservice/OnlineSavingAccountTypes?SEARCH_TYPE=ALL_ONLINE_SAVING</t>
   </si>
   <si>
     <t>{
-	"d": {
-		"Rate": "6.3",
-		"Term": "36M"
-	}
+    "d": {
+        "results": [
+            {
+                "__metadata": {
+                    "id": "https://smp-srv:8081/cb/odata/services/onlinesavingservice/OnlineSavingAccountTypes(1)",
+                    "uri": "https://smp-srv:8081/cb/odata/services/onlinesavingservice/OnlineSavingAccountTypes(1)",
+                    "type": "com.sap.banking.custom.onlinesaving.endpoint.v1_0.beans.OnlineSavingAccountType"
+                },
+                "Account_Type_ID": 1,
+                "Name_EN": "Tiết kiệm thường trực tuyến",
+                "Name_VN": "Tiết kiệm thường trực tuyến",
+                "Periodic": null,
+                "Tandc_Link": null,
+                "Status": "0",
+                "Introduce_product_name_en": "Enjoy interest based on the principal amount and flexible term",
+                "Introduce_product_name_vn": "Hưởng lãi suất theo số tiền gửi và kỳ hạn gửi đa dạng",
+                "Link_detail_product": "https://www.vpbank.com.vn/san-pham/gui-tiet-kiem/tiet-kiem-truc-tuyen"
+            },
+            {
+                "__metadata": {
+                    "id": "https://smp-srv:8081/cb/odata/services/onlinesavingservice/OnlineSavingAccountTypes(2)",
+                    "uri": "https://smp-srv:8081/cb/odata/services/onlinesavingservice/OnlineSavingAccountTypes(2)",
+                    "type": "com.sap.banking.custom.onlinesaving.endpoint.v1_0.beans.OnlineSavingAccountType"
+                },
+                "Account_Type_ID": 2,
+                "Name_EN": "Bảo toàn thịnh vượng trực tuyến",
+                "Name_VN": "Bảo toàn thịnh vượng trực tuyến",
+                "Periodic": null,
+                "Tandc_Link": null,
+                "Status": "0",
+                "Introduce_product_name_en": "Preserve interest rates before the fluctuations in interest rates on the market.",
+                "Introduce_product_name_vn": "Bảo toàn lãi suất trước những biến động lãi suất trên thị trường",
+                "Link_detail_product": "https://www.vpbank.com.vn/san-pham/gui-tiet-kiem/tiet-kiem-bao-toan-thinh-vuong"
+            },
+            {
+                "__metadata": {
+                    "id": "https://smp-srv:8081/cb/odata/services/onlinesavingservice/OnlineSavingAccountTypes(3)",
+                    "uri": "https://smp-srv:8081/cb/odata/services/onlinesavingservice/OnlineSavingAccountTypes(3)",
+                    "type": "com.sap.banking.custom.onlinesaving.endpoint.v1_0.beans.OnlineSavingAccountType"
+                },
+                "Account_Type_ID": 3,
+                "Name_EN": "Tiết kiệm lĩnh lãi định kỳ trực tuyến",
+                "Name_VN": "Tiết kiệm lĩnh lãi định kỳ trực tuyến",
+                "Periodic": null,
+                "Tandc_Link": null,
+                "Status": "0",
+                "Introduce_product_name_en": "Meet customers' demand for money using periodic interest",
+                "Introduce_product_name_vn": "Đáp ứng nhu cầu sử dụng tiền của Khách Hàng theo định kỳ lĩnh lãi",
+                "Link_detail_product": "https://www.vpbank.com.vn/san-pham/gui-tiet-kiem/tiet-kiem-linh-lai-dinh-ky"
+            },
+            {
+                "__metadata": {
+                    "id": "https://smp-srv:8081/cb/odata/services/onlinesavingservice/OnlineSavingAccountTypes(4)",
+                    "uri": "https://smp-srv:8081/cb/odata/services/onlinesavingservice/OnlineSavingAccountTypes(4)",
+                    "type": "com.sap.banking.custom.onlinesaving.endpoint.v1_0.beans.OnlineSavingAccountType"
+                },
+                "Account_Type_ID": 4,
+                "Name_EN": "Tiết kiệm easy saving trực tuyến",
+                "Name_VN": "Tiết kiệm easy saving trực tuyến",
+                "Periodic": null,
+                "Tandc_Link": null,
+                "Status": "0",
+                "Introduce_product_name_en": "Flexible and profitable submissions for small funds",
+                "Introduce_product_name_vn": "Gửi góp linh hoạt và sinh lời hiệu quả cho khoản tiền nhỏ nhàn rỗi.",
+                "Link_detail_product": "https://www.vpbank.com.vn/san-pham/gui-tiet-kiem/tiet-kiem-gui-gop-linh-hoat-easy-savings"
+            },
+            {
+                "__metadata": {
+                    "id": "https://smp-srv:8081/cb/odata/services/onlinesavingservice/OnlineSavingAccountTypes(5)",
+                    "uri": "https://smp-srv:8081/cb/odata/services/onlinesavingservice/OnlineSavingAccountTypes(5)",
+                    "type": "com.sap.banking.custom.onlinesaving.endpoint.v1_0.beans.OnlineSavingAccountType"
+                },
+                "Account_Type_ID": 5,
+                "Name_EN": "Tiết kiệm trả lãi trước trực tuyến",
+                "Name_VN": "Tiết kiệm trả lãi trước trực tuyến",
+                "Periodic": null,
+                "Tandc_Link": null,
+                "Status": "0",
+                "Introduce_product_name_en": "Customer will receive prepaid interest amount as soon as open saving",
+                "Introduce_product_name_vn": "Khách Hàng được nhận tiền lãi ngay khi gửi tiết kiệm",
+                "Link_detail_product": "https://www.vpbank.com.vn/san-pham/gui-tiet-kiem/tiet-kiem-tra-lai-truoc"
+            },
+            {
+                "__metadata": {
+                    "id": "https://smp-srv:8081/cb/odata/services/onlinesavingservice/OnlineSavingAccountTypes(6)",
+                    "uri": "https://smp-srv:8081/cb/odata/services/onlinesavingservice/OnlineSavingAccountTypes(6)",
+                    "type": "com.sap.banking.custom.onlinesaving.endpoint.v1_0.beans.OnlineSavingAccountType"
+                },
+                "Account_Type_ID": 6,
+                "Name_EN": "Tiết kiệm Phát Lộc Thịnh Vượng trực tuyến",
+                "Name_VN": "Tiết kiệm Phát Lộc Thịnh Vượng trực tuyến",
+                "Periodic": null,
+                "Tandc_Link": "http://www.vpbank.com.vn/",
+                "Status": "0",
+                "Introduce_product_name_en": null,
+                "Introduce_product_name_vn": null,
+                "Link_detail_product": null
+            },
+            {
+                "__metadata": {
+                    "id": "https://smp-srv:8081/cb/odata/services/onlinesavingservice/OnlineSavingAccountTypes(7)",
+                    "uri": "https://smp-srv:8081/cb/odata/services/onlinesavingservice/OnlineSavingAccountTypes(7)",
+                    "type": "com.sap.banking.custom.onlinesaving.endpoint.v1_0.beans.OnlineSavingAccountType"
+                },
+                "Account_Type_ID": 7,
+                "Name_EN": "Tiết kiệm bảo chứng thấu chi",
+                "Name_VN": "Tiết kiệm bảo chứng thấu chi",
+                "Periodic": null,
+                "Tandc_Link": "http://www.vpbank.com.vn/sites/default/files/pictures/Ti%E1%BA%BFt%20ki%E1%BB%87m%20th%C6%B0%E1%BB%9Dng.pdf",
+                "Status": "0",
+                "Introduce_product_name_en": "Combinations packgage of Online normal saving and secured overdraft product.",
+                "Introduce_product_name_vn": "Khách Hàng không cần tất toán trước hạn vẫn được sử dụng tiền ngay khi cần",
+                "Link_detail_product": "https://www.vpbank.com.vn/san-pham/gui-tiet-kiem/tiet-kiem-bao-chung-thau-chi"
+            }
+        ]
+    }
 }</t>
   </si>
 </sst>
@@ -773,8 +885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A4:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -918,7 +1030,9 @@
       <c r="H15" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="I15" s="15"/>
+      <c r="I15" s="15" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>

</xml_diff>